<commit_message>
chore(login): removed default values
</commit_message>
<xml_diff>
--- a/public/students_list.xlsx
+++ b/public/students_list.xlsx
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
     <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akshat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">akshat@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -114,16 +108,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -319,29 +317,25 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -349,9 +343,6 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="akshat@gmail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
feat(exporter): added female symbol in gazzet exporter
</commit_message>
<xml_diff>
--- a/public/students_list.xlsx
+++ b/public/students_list.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Students" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
     <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
   </si>
 </sst>
 </file>
@@ -39,7 +42,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -59,9 +62,10 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b val="true"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -108,20 +112,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -154,40 +150,40 @@
         <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285f4"/>
+        <a:srgbClr val="4f81bd"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ea4335"/>
+        <a:srgbClr val="c0504d"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="fbbc04"/>
+        <a:srgbClr val="9bbb59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34a853"/>
+        <a:srgbClr val="8064a2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="ff6d01"/>
+        <a:srgbClr val="4bacc6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46bdc6"/>
+        <a:srgbClr val="f79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155cc"/>
+        <a:srgbClr val="0000ff"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155cc"/>
+        <a:srgbClr val="0000ff"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Calibri" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Calibri" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -314,38 +310,1020 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C996"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:C7"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1"/>
-    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>